<commit_message>
Added student body demographics
</commit_message>
<xml_diff>
--- a/Formatted-Data/enrollment_statistics.xlsx
+++ b/Formatted-Data/enrollment_statistics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\Documents\alc\Formatted-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F99434-E7F3-4888-AD08-3E2BDE99B65C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09187308-B475-4FDA-8365-1980EFBB092E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{AC0BD6E1-1E93-43A4-8FE7-90504166469E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{AC0BD6E1-1E93-43A4-8FE7-90504166469E}"/>
   </bookViews>
   <sheets>
     <sheet name="Aggregated Enrollment Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Student Body Makeup" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="54">
   <si>
     <t>Notes</t>
   </si>
@@ -109,6 +110,90 @@
   </si>
   <si>
     <t>Data Type</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Other U.S.</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>Geographic Origin (%)</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Gender Balance (%)</t>
+  </si>
+  <si>
+    <t>Ethnic Diversity (%)</t>
+  </si>
+  <si>
+    <t>Two or more</t>
+  </si>
+  <si>
+    <t>African American</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Native American</t>
+  </si>
+  <si>
+    <t>Native Hawaiian/Pacific Islander</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Asian/Asian American was used interchangably by Stanford. A distiction cannot be made here.</t>
+  </si>
+  <si>
+    <t>Also listed as "Declined to State/Other" in some years</t>
+  </si>
+  <si>
+    <t>Also listed as "Hispanic/Latino" in some years</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>Stateless peoples are counted as "Other U.S."</t>
+  </si>
+  <si>
+    <t>The Americas</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Middle East and North Africa</t>
+  </si>
+  <si>
+    <t>Pacific Basin</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Geographic Origin (% of Foreign)</t>
+  </si>
+  <si>
+    <t>Measured in the Fall of each year, describes entire undergraduate class, data taken from https://facts.stanford.edu/academics/undergraduate-profile/ with past data retreived via the WayBack Machine (eg. https://web.archive.org/web/20130406141549/http://facts.stanford.edu/academics/undergraduate-profile)</t>
   </si>
 </sst>
 </file>
@@ -462,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B93501D-9FFD-431F-A6B0-5767EF8CA38F}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,4 +1469,653 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49858F93-0401-421B-94E2-CED0F42A9ED0}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>39</v>
+      </c>
+      <c r="E2">
+        <v>37.6</v>
+      </c>
+      <c r="F2">
+        <v>36</v>
+      </c>
+      <c r="G2">
+        <v>36</v>
+      </c>
+      <c r="H2">
+        <v>35</v>
+      </c>
+      <c r="I2">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>53</v>
+      </c>
+      <c r="D3">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <v>54.2</v>
+      </c>
+      <c r="F3">
+        <v>55.3</v>
+      </c>
+      <c r="G3">
+        <v>53</v>
+      </c>
+      <c r="H3">
+        <v>53</v>
+      </c>
+      <c r="I3">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>52</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <v>47.6</v>
+      </c>
+      <c r="F5">
+        <v>43.79</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F6">
+        <v>22.71</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="F7">
+        <v>16.34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>7.8</v>
+      </c>
+      <c r="F8">
+        <v>8.5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>5.2</v>
+      </c>
+      <c r="F9">
+        <v>6.05</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2.6</v>
+      </c>
+      <c r="F10">
+        <v>2.61</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11">
+        <v>48</v>
+      </c>
+      <c r="D11">
+        <v>47</v>
+      </c>
+      <c r="E11">
+        <v>47.2</v>
+      </c>
+      <c r="F11">
+        <v>47.6</v>
+      </c>
+      <c r="G11">
+        <v>48</v>
+      </c>
+      <c r="H11">
+        <v>50</v>
+      </c>
+      <c r="I11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>52</v>
+      </c>
+      <c r="D12">
+        <v>53</v>
+      </c>
+      <c r="E12">
+        <v>52.8</v>
+      </c>
+      <c r="F12">
+        <v>52.4</v>
+      </c>
+      <c r="G12">
+        <v>52</v>
+      </c>
+      <c r="H12">
+        <v>50</v>
+      </c>
+      <c r="I12">
+        <v>50</v>
+      </c>
+      <c r="J12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>7.5</v>
+      </c>
+      <c r="F13">
+        <v>7.8</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>21</v>
+      </c>
+      <c r="D14">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <v>22.6</v>
+      </c>
+      <c r="F14">
+        <v>22.9</v>
+      </c>
+      <c r="G14">
+        <v>21</v>
+      </c>
+      <c r="H14">
+        <v>22</v>
+      </c>
+      <c r="I14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F15">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>9</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2.1</v>
+      </c>
+      <c r="F16">
+        <v>1.9</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1.2</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0.5</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18">
+        <f>6+7</f>
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <f>7+7</f>
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <f>6.8+6.3</f>
+        <v>13.1</v>
+      </c>
+      <c r="F18">
+        <v>12.6</v>
+      </c>
+      <c r="G18">
+        <v>16</v>
+      </c>
+      <c r="H18">
+        <v>15</v>
+      </c>
+      <c r="I18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19">
+        <v>39</v>
+      </c>
+      <c r="D19">
+        <v>41</v>
+      </c>
+      <c r="E19">
+        <v>42.8</v>
+      </c>
+      <c r="F19">
+        <v>42.5</v>
+      </c>
+      <c r="G19">
+        <v>36</v>
+      </c>
+      <c r="H19">
+        <v>36</v>
+      </c>
+      <c r="I19">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>9</v>
+      </c>
+      <c r="I20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>2.6</v>
+      </c>
+      <c r="F21">
+        <v>2.5</v>
+      </c>
+      <c r="G21">
+        <v>0.5</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added issued student degree data
</commit_message>
<xml_diff>
--- a/Formatted-Data/enrollment_statistics.xlsx
+++ b/Formatted-Data/enrollment_statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\Documents\alc\Formatted-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09187308-B475-4FDA-8365-1980EFBB092E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9266B80-A1E7-4EB7-A606-2CC1E4F9BFDD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{AC0BD6E1-1E93-43A4-8FE7-90504166469E}"/>
   </bookViews>
@@ -1476,7 +1476,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>